<commit_message>
[IMP] re-arrange data mapping to templates
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_green_product_summary.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_green_product_summary.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neunghathai\Desktop\Report Pabi\รายการแก้ไข\Template Report Pabi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">วันที่ </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -56,23 +53,35 @@
     <t>ราคาต่อหน่วย</t>
   </si>
   <si>
-    <t>จำนวนเงิน (รวม VAT)</t>
-  </si>
-  <si>
     <t>สกุลเงิน</t>
   </si>
   <si>
     <t>แบบรายงานผลการจัดซื้อจัดจ้างและบริการที่เป็นมิตรกับสิ่งแวดล้อม</t>
+  </si>
+  <si>
+    <t>ศูนย์</t>
+  </si>
+  <si>
+    <t>จากวันที่</t>
+  </si>
+  <si>
+    <t>ถึงวันที่</t>
+  </si>
+  <si>
+    <t>ประเภทสินค้า</t>
+  </si>
+  <si>
+    <t>ภาษีมูลค่าเพิ่ม</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -86,27 +95,39 @@
     <font>
       <b/>
       <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Tahoma"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,54 +176,83 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,136 +535,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="6" customWidth="1"/>
-    <col min="2" max="5" width="20" style="6" customWidth="1"/>
-    <col min="6" max="10" width="17.33203125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="10" customWidth="1"/>
-    <col min="12" max="13" width="11.83203125" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="12" style="10" customWidth="1"/>
+    <col min="2" max="2" width="16" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16" style="10" customWidth="1"/>
+    <col min="4" max="4" width="31.54296875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="17" customWidth="1"/>
+    <col min="7" max="8" width="17.7265625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="17.36328125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="17.36328125" style="10" customWidth="1"/>
+    <col min="12" max="13" width="11.81640625" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="4"/>
-    </row>
-    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="7" spans="1:14" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="6" spans="1:14" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="B7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="C7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="E7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="G7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="H7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="8" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="9" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="17" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="18" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="19" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="20" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    </row>
+    <row r="8" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="22"/>
+    </row>
+    <row r="12" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="22"/>
+    </row>
+    <row r="15" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="22"/>
+    </row>
+    <row r="17" spans="1:9" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="22"/>
+    </row>
+    <row r="18" spans="1:9" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="22"/>
+    </row>
+    <row r="19" spans="1:9" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="22"/>
+    </row>
+    <row r="20" spans="1:9" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="22"/>
+    </row>
+    <row r="21" spans="1:9" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.60972222222222205" bottom="0.37013888888888902" header="0.51180555555555496" footer="0.1"/>

</xml_diff>

<commit_message>
[ENH] rework on reports
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_green_product_summary.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_green_product_summary.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neunghathai\Desktop\Report Pabi\รายการแก้ไข\Template Report Pabi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -72,12 +72,18 @@
   </si>
   <si>
     <t>ภาษีมูลค่าเพิ่ม</t>
+  </si>
+  <si>
+    <t>Green  Product</t>
+  </si>
+  <si>
+    <t>Innovation Product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
@@ -244,13 +250,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -538,32 +544,32 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" style="10" customWidth="1"/>
     <col min="2" max="2" width="16" style="8" customWidth="1"/>
     <col min="3" max="3" width="16" style="10" customWidth="1"/>
-    <col min="4" max="4" width="31.54296875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" style="17" customWidth="1"/>
-    <col min="7" max="8" width="17.7265625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="17.7265625" style="14" customWidth="1"/>
-    <col min="10" max="10" width="17.36328125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="17.36328125" style="10" customWidth="1"/>
-    <col min="12" max="13" width="11.81640625" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="8.81640625" style="11"/>
+    <col min="4" max="4" width="31.5" style="8" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="17" customWidth="1"/>
+    <col min="7" max="8" width="17.6640625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="10" customWidth="1"/>
+    <col min="12" max="13" width="11.83203125" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="2"/>
       <c r="F1" s="15"/>
       <c r="G1" s="1"/>
@@ -575,8 +581,8 @@
       <c r="M1" s="2"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="7"/>
@@ -593,8 +599,8 @@
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="7"/>
@@ -611,8 +617,8 @@
       <c r="M3" s="6"/>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="7"/>
@@ -629,8 +635,8 @@
       <c r="M4" s="6"/>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+    <row r="5" spans="1:14" s="4" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="7"/>
@@ -647,7 +653,7 @@
       <c r="M5" s="6"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="7" spans="1:14" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
         <v>0</v>
       </c>
@@ -675,8 +681,14 @@
       <c r="I7" s="18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="20"/>
       <c r="B8" s="22"/>
       <c r="C8" s="20"/>
@@ -686,7 +698,7 @@
       <c r="H8" s="20"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="20"/>
       <c r="B9" s="22"/>
       <c r="C9" s="20"/>
@@ -696,7 +708,7 @@
       <c r="H9" s="20"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="20"/>
       <c r="B10" s="22"/>
       <c r="C10" s="20"/>
@@ -706,7 +718,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="20"/>
       <c r="B11" s="22"/>
       <c r="C11" s="20"/>
@@ -716,7 +728,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="20"/>
       <c r="B12" s="22"/>
       <c r="C12" s="20"/>
@@ -726,7 +738,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="20"/>
       <c r="B13" s="22"/>
       <c r="C13" s="20"/>
@@ -736,7 +748,7 @@
       <c r="H13" s="20"/>
       <c r="I13" s="22"/>
     </row>
-    <row r="14" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="20"/>
       <c r="B14" s="22"/>
       <c r="C14" s="20"/>
@@ -746,7 +758,7 @@
       <c r="H14" s="20"/>
       <c r="I14" s="22"/>
     </row>
-    <row r="15" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="20"/>
       <c r="B15" s="22"/>
       <c r="C15" s="20"/>
@@ -756,7 +768,7 @@
       <c r="H15" s="20"/>
       <c r="I15" s="22"/>
     </row>
-    <row r="16" spans="1:14" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="20"/>
       <c r="B16" s="22"/>
       <c r="C16" s="20"/>
@@ -766,7 +778,7 @@
       <c r="H16" s="20"/>
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="1:9" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="20"/>
       <c r="B17" s="22"/>
       <c r="C17" s="20"/>
@@ -776,7 +788,7 @@
       <c r="H17" s="20"/>
       <c r="I17" s="22"/>
     </row>
-    <row r="18" spans="1:9" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="20"/>
       <c r="B18" s="22"/>
       <c r="C18" s="20"/>
@@ -786,7 +798,7 @@
       <c r="H18" s="20"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:9" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="20"/>
       <c r="B19" s="22"/>
       <c r="C19" s="20"/>
@@ -796,7 +808,7 @@
       <c r="H19" s="20"/>
       <c r="I19" s="22"/>
     </row>
-    <row r="20" spans="1:9" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="20"/>
       <c r="B20" s="22"/>
       <c r="C20" s="20"/>
@@ -806,7 +818,7 @@
       <c r="H20" s="20"/>
       <c r="I20" s="22"/>
     </row>
-    <row r="21" spans="1:9" s="21" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="20"/>
       <c r="B21" s="22"/>
       <c r="C21" s="20"/>

</xml_diff>